<commit_message>
checked aero drag sheet
</commit_message>
<xml_diff>
--- a/examples/0_analyses_of_ref_vehicle/1_aerodynamic_analysis/estimate_aero_drag.xlsx
+++ b/examples/0_analyses_of_ref_vehicle/1_aerodynamic_analysis/estimate_aero_drag.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/examples/analyses_of_ref_vehicle/1_aerodynamic_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/examples/0_analyses_of_ref_vehicle/1_aerodynamic_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3A515D-8615-B143-824C-66EF624D9077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35045786-2E33-874D-809E-1B09DAEC9D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" activeTab="1" xr2:uid="{5EC0E62E-FE45-5247-ADB4-6FC5840AA93C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{5EC0E62E-FE45-5247-ADB4-6FC5840AA93C}"/>
   </bookViews>
   <sheets>
     <sheet name="multirotor" sheetId="3" r:id="rId1"/>
@@ -380,35 +380,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2914,95 +2913,89 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="12.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="3"/>
-    <col min="6" max="6" width="5.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="3" customWidth="1"/>
-    <col min="8" max="9" width="12.83203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="24" style="3" customWidth="1"/>
-    <col min="11" max="14" width="10.83203125" style="3"/>
-    <col min="15" max="15" width="14.33203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="15" style="3" customWidth="1"/>
-    <col min="17" max="18" width="13.5" style="3" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" style="3"/>
-    <col min="20" max="20" width="10" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="3"/>
-    <col min="22" max="22" width="10.5" style="3" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="18" width="13.5" customWidth="1"/>
+    <col min="20" max="20" width="10" customWidth="1"/>
+    <col min="22" max="22" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <f>PI()*C30*C30</f>
         <v>55.582486455932631</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>50</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1">
@@ -3069,13 +3062,13 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>1524</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="1">
@@ -3142,13 +3135,13 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>278.24399999999901</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1">
@@ -3215,13 +3208,13 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1">
@@ -3288,13 +3281,13 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>84314.678467682505</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1">
@@ -3361,13 +3354,13 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>1.05563913070961</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1"/>
@@ -3388,34 +3381,34 @@
       <c r="V8" s="1"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>1.4</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N9" s="1"/>
@@ -3428,13 +3421,13 @@
       <c r="V9" s="1"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>1.7411824005015001E-5</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="1">
@@ -3474,14 +3467,14 @@
       <c r="V10" s="1"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <f>C8*C3/C10</f>
         <v>3031385.8284047726</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="1">
@@ -3522,10 +3515,10 @@
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <f>C3/334.512939421475</f>
         <v>0.14947104912136655</v>
       </c>
@@ -3643,7 +3636,7 @@
       <c r="V14" s="1"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="1">
@@ -3684,13 +3677,13 @@
       <c r="V15" s="1"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>6.4008000000000003</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="1"/>
@@ -3712,13 +3705,13 @@
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>2.0560284000000002</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="F17" s="1"/>
@@ -3740,10 +3733,10 @@
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="6"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="1">
         <f>T3</f>
         <v>0.12826124605494557</v>
@@ -3751,7 +3744,7 @@
       <c r="I18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J18" s="8"/>
+      <c r="J18" s="6"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -3766,13 +3759,13 @@
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="6"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="1">
         <f>SUM(T4:T7)</f>
         <v>0.44160171008627935</v>
@@ -3788,17 +3781,17 @@
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <f>(0.2+0.2+0.36)/3</f>
         <v>0.25333333333333335</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="1">
         <f>SUM(K10:K15)</f>
         <v>8.4038282200000008E-2</v>
@@ -3811,19 +3804,19 @@
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>7.4333200000000001</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="1">
         <f>SUM(T3:T7)+SUM(K10:K15)</f>
         <v>0.65390123834122482</v>
@@ -3836,21 +3829,21 @@
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22">
         <v>4.3058100000000001</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G22" s="6"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="1">
         <f>SUM(U3:U7)+SUM(L10:L15)</f>
         <v>1.1764519366359335E-2</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="5"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -3859,7 +3852,7 @@
       <c r="U22" s="1"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="G23" s="3" t="s">
+      <c r="G23" t="s">
         <v>59</v>
       </c>
       <c r="H23" s="1">
@@ -3874,7 +3867,7 @@
       <c r="U23" s="1"/>
     </row>
     <row r="24" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>68</v>
       </c>
       <c r="P24" s="1"/>
@@ -3885,10 +3878,10 @@
       <c r="U24" s="1"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25">
         <f>(0.27273+0.27273+0.2+0.32)/4</f>
         <v>0.26636500000000002</v>
       </c>
@@ -3901,21 +3894,21 @@
       <c r="V25" s="1"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
+      <c r="B26" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26">
         <v>6.5445599999999997</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -3925,22 +3918,22 @@
       <c r="V26" s="1"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27">
         <v>4.5923299999999996</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="P27" s="1"/>
@@ -3971,7 +3964,7 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F29" s="1">
@@ -3993,13 +3986,13 @@
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
+      <c r="B30" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30">
         <v>4.2062400000000002</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="F30" s="1">
@@ -4022,7 +4015,7 @@
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="F31" s="1"/>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="7" t="s">
         <v>63</v>
       </c>
       <c r="H31" s="1">
@@ -4035,15 +4028,15 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="5"/>
-      <c r="G33" s="4" t="s">
+      <c r="B33" s="4"/>
+      <c r="G33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="8">
         <f>H31*C2*0.5*C8*C3^2</f>
         <v>862.8546685155851</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4067,101 +4060,95 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C26355C-190F-DE43-B836-7F66296BD012}">
   <dimension ref="B2:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="3"/>
-    <col min="6" max="6" width="5.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="3" customWidth="1"/>
-    <col min="8" max="9" width="12.83203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="24" style="3" customWidth="1"/>
-    <col min="11" max="14" width="10.83203125" style="3"/>
-    <col min="15" max="15" width="14.33203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="15" style="3" customWidth="1"/>
-    <col min="17" max="18" width="13.5" style="3" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" style="3"/>
-    <col min="20" max="20" width="10" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="3"/>
-    <col min="22" max="22" width="10.5" style="3" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="18" width="13.5" customWidth="1"/>
+    <col min="20" max="20" width="10" customWidth="1"/>
+    <col min="22" max="22" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>19.535478449999999</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>50</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1">
@@ -4228,13 +4215,13 @@
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>1524</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="1">
@@ -4300,13 +4287,13 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>278.24399999999901</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1">
@@ -4372,13 +4359,13 @@
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1">
@@ -4444,13 +4431,13 @@
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>84314.678467682505</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1">
@@ -4517,13 +4504,13 @@
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>1.05563913070961</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1">
@@ -4590,10 +4577,10 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>1.4</v>
       </c>
       <c r="F9" s="1">
@@ -4660,13 +4647,13 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>1.7411824005015001E-5</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="1">
@@ -4733,14 +4720,14 @@
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <f>C8*C3/C10</f>
         <v>3031385.8284047726</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="1"/>
@@ -4761,35 +4748,35 @@
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <f>C3/334.512939421475</f>
         <v>0.14947104912136655</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N12" s="1"/>
@@ -4877,7 +4864,7 @@
       <c r="V14" s="1"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="1">
@@ -4918,13 +4905,13 @@
       <c r="V15" s="1"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>9.1440000000000001</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="1">
@@ -4965,13 +4952,13 @@
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>1.8675309360000001</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="F17" s="1">
@@ -5050,7 +5037,7 @@
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F19" s="1"/>
@@ -5072,19 +5059,19 @@
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <v>4.8768000000000002</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="1">
         <f>T3</f>
         <v>0.10361800681723543</v>
@@ -5107,19 +5094,19 @@
       <c r="V20" s="1"/>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>0.30480000000000002</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="1">
         <f>T4</f>
         <v>0.18671880490759174</v>
@@ -5127,7 +5114,7 @@
       <c r="I21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="8"/>
+      <c r="J21" s="6"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -5142,10 +5129,10 @@
       <c r="V21" s="1"/>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="6"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="1">
         <f>T5</f>
         <v>3.7277310018780707E-2</v>
@@ -5161,13 +5148,13 @@
       <c r="V22" s="1"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="6"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="1">
         <f>T6</f>
         <v>2.420824019086151E-2</v>
@@ -5180,19 +5167,19 @@
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+      <c r="B24" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24">
         <v>19.535478449999999</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G24" s="6"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="1">
         <f>SUM(T7:T10)</f>
         <v>6.4345556098475282E-2</v>
@@ -5205,19 +5192,19 @@
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+      <c r="B25" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25">
         <v>12.127610000000001</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="6"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="1">
         <f>SUM(K13:K18)</f>
         <v>5.2489398E-2</v>
@@ -5233,10 +5220,10 @@
       <c r="U25" s="1"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="6"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="1">
         <f>SUM(T3:T10) + SUM(K13:K18)</f>
         <v>0.46865731603294475</v>
@@ -5252,18 +5239,18 @@
       <c r="U26" s="1"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="6"/>
+      <c r="G27" s="9"/>
       <c r="H27" s="1">
         <f>SUM(U3:U10)+SUM(L13:L18)</f>
         <v>2.3990060813327285E-2</v>
       </c>
-      <c r="I27" s="7"/>
+      <c r="I27" s="5"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -5272,16 +5259,16 @@
       <c r="U27" s="1"/>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
+      <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28">
         <v>3.6707105940479998</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" t="s">
         <v>59</v>
       </c>
       <c r="H28" s="1">
@@ -5297,13 +5284,13 @@
       <c r="V28" s="1"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B29" s="3" t="s">
+      <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29">
         <v>4.3036300000000001</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" t="s">
         <v>5</v>
       </c>
       <c r="P29" s="1"/>
@@ -5324,39 +5311,39 @@
       <c r="V30" s="1"/>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
+      <c r="B32" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32">
         <v>2.5402710484800002</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="3" t="s">
         <v>25</v>
       </c>
       <c r="P32" s="1"/>
@@ -5364,13 +5351,13 @@
       <c r="R32" s="1"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
+      <c r="B33" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33">
         <v>1.1798999999999999</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" t="s">
         <v>5</v>
       </c>
       <c r="F33" s="1">
@@ -5473,7 +5460,7 @@
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.2">
       <c r="F39" s="1"/>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="7" t="s">
         <v>63</v>
       </c>
       <c r="H39" s="1">
@@ -5487,14 +5474,14 @@
     </row>
     <row r="40" spans="2:18" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="8">
         <f>H39*C2*0.5*C8*C3^2</f>
         <v>618.41625212214581</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="I41" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>